<commit_message>
Updated strings for translation
For Alt Controller v1.94
</commit_message>
<xml_diff>
--- a/AltController/Translation/Strings_for_translation.xlsx
+++ b/AltController/Translation/Strings_for_translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="1085">
   <si>
     <t xml:space="preserve">String_ID</t>
   </si>
@@ -2359,6 +2359,18 @@
     <t xml:space="preserve">Refresh the list of running programs</t>
   </si>
   <si>
+    <t xml:space="preserve">Situations_SnoozeLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snooze profile when using this app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Situations_SnoozeToolTip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't perform any actions while this app is active</t>
+  </si>
+  <si>
     <t xml:space="preserve">Situations_Title</t>
   </si>
   <si>
@@ -3077,6 +3089,12 @@
   </si>
   <si>
     <t xml:space="preserve">Situation Changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_snooze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snooze</t>
   </si>
   <si>
     <t xml:space="preserve">String_Standard_pointer</t>
@@ -3364,13 +3382,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D530"/>
+  <dimension ref="A1:D533"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D117" activeCellId="0" sqref="A117:D117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D503" activeCellId="0" sqref="A503:D503"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.75"/>
@@ -7558,29 +7576,29 @@
         <v>749</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>749</v>
+        <v>780</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>133</v>
+        <v>749</v>
       </c>
       <c r="D381" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>133</v>
+        <v>749</v>
       </c>
       <c r="D382" s="0" t="s">
-        <v>783</v>
+        <v>749</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8218,29 +8236,29 @@
         <v>133</v>
       </c>
       <c r="D440" s="0" t="s">
-        <v>515</v>
+        <v>899</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C441" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D441" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C442" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D442" s="0" t="s">
-        <v>902</v>
+        <v>515</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8944,40 +8962,40 @@
         <v>133</v>
       </c>
       <c r="D506" s="0" t="s">
-        <v>45</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C507" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D507" s="0" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C508" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D508" s="0" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C509" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D509" s="0" t="s">
-        <v>1035</v>
+        <v>45</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9205,10 +9223,43 @@
         <v>1076</v>
       </c>
       <c r="C530" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D530" s="0" t="s">
         <v>1077</v>
       </c>
-      <c r="D530" s="0" t="s">
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="0" t="s">
         <v>1078</v>
+      </c>
+      <c r="C531" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D531" s="0" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C532" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D532" s="0" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="0" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C533" s="0" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D533" s="0" t="s">
+        <v>1084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised window action types.
</commit_message>
<xml_diff>
--- a/AltController/Translation/Strings_for_translation.xlsx
+++ b/AltController/Translation/Strings_for_translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="1306">
   <si>
     <t xml:space="preserve">String_ID</t>
   </si>
@@ -130,6 +130,12 @@
     <t xml:space="preserve">Edit action - Move pointer</t>
   </si>
   <si>
+    <t xml:space="preserve">Action_ActionLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Action_ActionTypeLabel</t>
   </si>
   <si>
@@ -709,12 +715,6 @@
     <t xml:space="preserve">Error while changing the action type</t>
   </si>
   <si>
-    <t xml:space="preserve">E_ChangeProfileUnsavedChanges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unable to change profile because the current profile has unsaved changes.</t>
-  </si>
-  <si>
     <t xml:space="preserve">E_CommandEmpty</t>
   </si>
   <si>
@@ -877,112 +877,130 @@
     <t xml:space="preserve">Invalid regular expression.</t>
   </si>
   <si>
-    <t xml:space="preserve">E_LoadProfileAction</t>
+    <t xml:space="preserve">E_MAIN001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while initialising folders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while initialising application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while positioning window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while creating new profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while saving profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error during Save As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening the profile editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening the screen region editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening the profile summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while loading profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening all custom windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error during open custom window command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening custom window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while opening the Log information window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while loading recent profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while running command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN018</t>
   </si>
   <si>
     <t xml:space="preserve">Error performing load profile action.</t>
   </si>
   <si>
-    <t xml:space="preserve">E_MAIN001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while initialising folders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while initialising application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while positioning window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while creating new profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while saving profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error during Save As</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening the profile editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening the screen region editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening the profile summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while loading profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening all custom windows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error during open custom window command</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening custom window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while opening the Log information window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while loading recent profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_MAIN017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error while running command</t>
+    <t xml:space="preserve">E_MAIN019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot change profile when the profile editor is open.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot change profile when there are unsaved changes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_MAIN021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error running command</t>
   </si>
   <si>
     <t xml:space="preserve">E_PR001</t>
@@ -1273,12 +1291,6 @@
     <t xml:space="preserve">Error: selection of multiple regions is not allowed</t>
   </si>
   <si>
-    <t xml:space="preserve">E_RunCommand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error running command</t>
-  </si>
-  <si>
     <t xml:space="preserve">E_UPGR001</t>
   </si>
   <si>
@@ -2029,7 +2041,7 @@
     <t xml:space="preserve">Options_SecurityTab</t>
   </si>
   <si>
-    <t xml:space="preserve">Security</t>
+    <t xml:space="preserve">Sec_urity</t>
   </si>
   <si>
     <t xml:space="preserve">Options_ShiftCheck</t>
@@ -2995,12 +3007,36 @@
     <t xml:space="preserve">Executable files</t>
   </si>
   <si>
+    <t xml:space="preserve">String_Hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide</t>
+  </si>
+  <si>
     <t xml:space="preserve">String_Hide_pointer</t>
   </si>
   <si>
     <t xml:space="preserve">Hide pointer</t>
   </si>
   <si>
+    <t xml:space="preserve">String_HideAllCustomWindows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide all custom windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_HideCustomWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide custom window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_HideCustomWindowX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide custom window '{0}'</t>
+  </si>
+  <si>
     <t xml:space="preserve">String_Hold_down_key_for_X</t>
   </si>
   <si>
@@ -3139,6 +3175,24 @@
     <t xml:space="preserve">longer presses towards</t>
   </si>
   <si>
+    <t xml:space="preserve">String_Maximise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_MaximiseOrMinimiseWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximise / minimise window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_MaximiseOrRestore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximise / restore</t>
+  </si>
+  <si>
     <t xml:space="preserve">String_MaximiseOrRestoreWindow</t>
   </si>
   <si>
@@ -3163,10 +3217,10 @@
     <t xml:space="preserve">Middle</t>
   </si>
   <si>
-    <t xml:space="preserve">String_minimise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minimise</t>
+    <t xml:space="preserve">String_Minimise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimise</t>
   </si>
   <si>
     <t xml:space="preserve">String_MinimiseWindow</t>
@@ -3508,10 +3562,10 @@
     <t xml:space="preserve">Reset all options?</t>
   </si>
   <si>
-    <t xml:space="preserve">String_restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restore</t>
+    <t xml:space="preserve">String_Restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore</t>
   </si>
   <si>
     <t xml:space="preserve">String_Restore_pointer</t>
@@ -3593,6 +3647,54 @@
   </si>
   <si>
     <t xml:space="preserve">sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowAllCustomWindows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show all custom windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowCustomWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show custom window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowCustomWindowX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show custom window '{0}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowOrHide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show / hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowOrHideAllCustomWindows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show / hide all custom windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowOrHideCustomWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show / hide custom window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String_ShowOrHideCustomWindowX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show / hide custom window '{0}'</t>
   </si>
   <si>
     <t xml:space="preserve">String_Situation_Changed</t>
@@ -4053,10 +4155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D628"/>
+  <dimension ref="A1:D645"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A587" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C586" activeCellId="0" sqref="C586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4217,30 +4319,27 @@
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4251,29 +4350,29 @@
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4284,18 +4383,18 @@
         <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,40 +4405,40 @@
         <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4350,29 +4449,29 @@
         <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4383,29 +4482,29 @@
         <v>77</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4416,7 +4515,7 @@
         <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,18 +4526,18 @@
         <v>87</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,7 +4559,7 @@
         <v>94</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4471,18 +4570,18 @@
         <v>96</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4493,7 +4592,7 @@
         <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4504,7 +4603,7 @@
         <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,7 +4625,7 @@
         <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4537,7 +4636,7 @@
         <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4548,7 +4647,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4559,7 +4658,7 @@
         <v>113</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4570,7 +4669,7 @@
         <v>115</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4581,7 +4680,7 @@
         <v>117</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4592,7 +4691,7 @@
         <v>119</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4603,7 +4702,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,7 +4713,7 @@
         <v>123</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4625,7 +4724,7 @@
         <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,7 +4735,7 @@
         <v>127</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4647,7 +4746,7 @@
         <v>129</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4658,7 +4757,7 @@
         <v>131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,7 +4768,7 @@
         <v>133</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4779,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4691,18 +4790,18 @@
         <v>137</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4713,7 +4812,7 @@
         <v>142</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4721,21 +4820,21 @@
         <v>143</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4746,7 +4845,7 @@
         <v>147</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4768,18 +4867,18 @@
         <v>151</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4790,7 +4889,7 @@
         <v>156</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4801,7 +4900,7 @@
         <v>158</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,6 +4921,9 @@
       <c r="B73" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C73" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -4838,19 +4940,16 @@
       <c r="B75" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +4960,7 @@
         <v>171</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4872,7 +4971,7 @@
         <v>173</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4883,7 +4982,7 @@
         <v>175</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4894,7 +4993,7 @@
         <v>177</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,7 +5004,7 @@
         <v>179</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4916,7 +5015,7 @@
         <v>181</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4927,7 +5026,7 @@
         <v>183</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,7 +5037,7 @@
         <v>185</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4949,7 +5048,7 @@
         <v>187</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4960,7 +5059,7 @@
         <v>189</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4971,7 +5070,7 @@
         <v>191</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4982,7 +5081,7 @@
         <v>193</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4993,7 +5092,7 @@
         <v>195</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5004,7 +5103,7 @@
         <v>197</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5015,7 +5114,7 @@
         <v>199</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5026,7 +5125,7 @@
         <v>201</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5037,7 +5136,7 @@
         <v>203</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5048,7 +5147,7 @@
         <v>205</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5059,7 +5158,7 @@
         <v>207</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5070,7 +5169,7 @@
         <v>209</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5081,7 +5180,7 @@
         <v>211</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5092,7 +5191,7 @@
         <v>213</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,7 +5202,7 @@
         <v>215</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5114,7 +5213,7 @@
         <v>217</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,32 +5221,32 @@
         <v>218</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,32 +5254,32 @@
         <v>222</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5188,18 +5287,21 @@
         <v>226</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>228</v>
+        <v>201</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5993,30 +6095,24 @@
       <c r="B207" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C207" s="1" t="s">
-        <v>427</v>
-      </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="C209" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6027,7 +6123,7 @@
         <v>433</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6038,7 +6134,7 @@
         <v>435</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6046,21 +6142,21 @@
         <v>436</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6071,7 +6167,7 @@
         <v>431</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6082,18 +6178,18 @@
         <v>442</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6104,7 +6200,7 @@
         <v>446</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6115,29 +6211,29 @@
         <v>448</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B219" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="C219" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="C220" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6148,7 +6244,7 @@
         <v>455</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6159,7 +6255,7 @@
         <v>457</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6170,7 +6266,7 @@
         <v>459</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6181,7 +6277,7 @@
         <v>461</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6192,7 +6288,7 @@
         <v>463</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6203,7 +6299,7 @@
         <v>465</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,7 +6310,7 @@
         <v>467</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6225,7 +6321,7 @@
         <v>469</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6235,6 +6331,9 @@
       <c r="B229" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="C229" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
@@ -6243,6 +6342,9 @@
       <c r="B230" s="1" t="s">
         <v>473</v>
       </c>
+      <c r="C230" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
@@ -6297,23 +6399,23 @@
         <v>486</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>164</v>
+        <v>487</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>490</v>
+        <v>166</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6627,26 +6729,23 @@
       <c r="B278" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C278" s="1" t="s">
-        <v>569</v>
-      </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B279" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="B279" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="C279" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B280" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="C280" s="1" t="s">
         <v>573</v>
       </c>
     </row>
@@ -6658,51 +6757,48 @@
         <v>575</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B282" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="B282" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C283" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C284" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="C284" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B285" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="B285" s="1" t="s">
+      <c r="C285" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6713,7 +6809,7 @@
         <v>588</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6724,51 +6820,51 @@
         <v>590</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B288" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B288" s="1" t="s">
-        <v>593</v>
-      </c>
       <c r="C288" s="1" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B289" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="B289" s="1" t="s">
+      <c r="C289" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B290" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="B290" s="1" t="s">
-        <v>598</v>
-      </c>
       <c r="C290" s="1" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B291" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="C291" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6779,7 +6875,7 @@
         <v>602</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6790,7 +6886,7 @@
         <v>604</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6801,7 +6897,7 @@
         <v>606</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>582</v>
+        <v>600</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6812,7 +6908,7 @@
         <v>608</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>582</v>
+        <v>600</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6823,7 +6919,7 @@
         <v>610</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6834,7 +6930,7 @@
         <v>612</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6845,7 +6941,7 @@
         <v>614</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6856,29 +6952,29 @@
         <v>616</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>617</v>
+        <v>586</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B300" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="B300" s="1" t="s">
-        <v>619</v>
-      </c>
       <c r="C300" s="1" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B301" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="B301" s="1" t="s">
+      <c r="C301" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6889,7 +6985,7 @@
         <v>623</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6900,7 +6996,7 @@
         <v>625</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6911,7 +7007,7 @@
         <v>627</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>576</v>
+        <v>595</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6922,7 +7018,7 @@
         <v>629</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6933,7 +7029,7 @@
         <v>631</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6944,7 +7040,7 @@
         <v>633</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>617</v>
+        <v>583</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6955,7 +7051,7 @@
         <v>635</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6966,7 +7062,7 @@
         <v>637</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6977,7 +7073,7 @@
         <v>639</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6988,7 +7084,7 @@
         <v>641</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6999,7 +7095,7 @@
         <v>643</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7010,7 +7106,7 @@
         <v>645</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7021,7 +7117,7 @@
         <v>647</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7032,7 +7128,7 @@
         <v>649</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7043,7 +7139,7 @@
         <v>651</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7054,7 +7150,7 @@
         <v>653</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7065,29 +7161,29 @@
         <v>655</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>656</v>
+        <v>600</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B319" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="B319" s="1" t="s">
-        <v>658</v>
-      </c>
       <c r="C319" s="1" t="s">
-        <v>656</v>
+        <v>600</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B320" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="B320" s="1" t="s">
+      <c r="C320" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="C320" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7098,29 +7194,29 @@
         <v>662</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="B322" s="1" t="s">
-        <v>665</v>
-      </c>
       <c r="C322" s="1" t="s">
-        <v>663</v>
+        <v>586</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B323" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B323" s="1" t="s">
+      <c r="C323" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="C323" s="1" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7131,7 +7227,7 @@
         <v>669</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7142,7 +7238,7 @@
         <v>671</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>579</v>
+        <v>667</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7153,7 +7249,7 @@
         <v>673</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>582</v>
+        <v>667</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7164,7 +7260,7 @@
         <v>675</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>617</v>
+        <v>583</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7175,7 +7271,7 @@
         <v>677</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>656</v>
+        <v>586</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7186,7 +7282,7 @@
         <v>679</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7197,7 +7293,7 @@
         <v>681</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>576</v>
+        <v>660</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7208,7 +7304,7 @@
         <v>683</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>576</v>
+        <v>621</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7219,7 +7315,7 @@
         <v>685</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7230,7 +7326,7 @@
         <v>687</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>687</v>
+        <v>580</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7241,29 +7337,29 @@
         <v>689</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>690</v>
+        <v>583</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B335" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="B335" s="1" t="s">
-        <v>692</v>
-      </c>
       <c r="C335" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B336" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="B336" s="1" t="s">
+      <c r="C336" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7274,7 +7370,7 @@
         <v>696</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7285,7 +7381,7 @@
         <v>698</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7296,7 +7392,7 @@
         <v>700</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7307,7 +7403,7 @@
         <v>702</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7318,7 +7414,7 @@
         <v>704</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7329,7 +7425,7 @@
         <v>706</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7340,7 +7436,7 @@
         <v>708</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7351,7 +7447,7 @@
         <v>710</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7362,7 +7458,7 @@
         <v>712</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7373,7 +7469,7 @@
         <v>714</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7384,7 +7480,7 @@
         <v>716</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7395,7 +7491,7 @@
         <v>718</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7406,7 +7502,7 @@
         <v>720</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7417,7 +7513,7 @@
         <v>722</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7428,7 +7524,7 @@
         <v>724</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7439,7 +7535,7 @@
         <v>726</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7450,7 +7546,7 @@
         <v>728</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7461,7 +7557,7 @@
         <v>730</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7472,7 +7568,7 @@
         <v>732</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7483,7 +7579,7 @@
         <v>734</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7494,7 +7590,7 @@
         <v>736</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7505,7 +7601,7 @@
         <v>738</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7516,7 +7612,7 @@
         <v>740</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7524,21 +7620,21 @@
         <v>741</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>690</v>
+        <v>742</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>744</v>
+        <v>694</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7546,21 +7642,21 @@
         <v>745</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>746</v>
+        <v>694</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>744</v>
+        <v>694</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B363" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="C363" s="1" t="s">
         <v>748</v>
-      </c>
-      <c r="C363" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7571,7 +7667,7 @@
         <v>750</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7579,10 +7675,10 @@
         <v>751</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>438</v>
+        <v>752</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7593,7 +7689,7 @@
         <v>754</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7601,43 +7697,43 @@
         <v>755</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>173</v>
+        <v>442</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C368" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="B368" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C368" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>758</v>
+        <v>175</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>760</v>
+        <v>171</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7648,7 +7744,7 @@
         <v>762</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7659,7 +7755,7 @@
         <v>764</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7670,7 +7766,7 @@
         <v>766</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7678,32 +7774,32 @@
         <v>767</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>431</v>
+        <v>768</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>771</v>
+        <v>435</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7714,7 +7810,7 @@
         <v>773</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7725,7 +7821,7 @@
         <v>775</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7736,7 +7832,7 @@
         <v>777</v>
       </c>
       <c r="C379" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7747,7 +7843,7 @@
         <v>779</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7758,7 +7854,7 @@
         <v>781</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7769,7 +7865,7 @@
         <v>783</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7780,7 +7876,7 @@
         <v>785</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7791,7 +7887,7 @@
         <v>787</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7802,7 +7898,7 @@
         <v>789</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7813,7 +7909,7 @@
         <v>791</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7824,7 +7920,7 @@
         <v>793</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7835,7 +7931,7 @@
         <v>795</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7846,7 +7942,7 @@
         <v>797</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7857,7 +7953,7 @@
         <v>799</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7868,7 +7964,7 @@
         <v>801</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7879,7 +7975,7 @@
         <v>803</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7890,7 +7986,7 @@
         <v>805</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,7 +7997,7 @@
         <v>807</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7912,7 +8008,7 @@
         <v>809</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7923,7 +8019,7 @@
         <v>811</v>
       </c>
       <c r="C396" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7931,54 +8027,54 @@
         <v>812</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>752</v>
+        <v>813</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>197</v>
+        <v>756</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>426</v>
+        <v>199</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>819</v>
+        <v>756</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7989,7 +8085,7 @@
         <v>821</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>819</v>
+        <v>756</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7997,10 +8093,10 @@
         <v>822</v>
       </c>
       <c r="B403" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C403" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="C403" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8011,7 +8107,7 @@
         <v>825</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8022,7 +8118,7 @@
         <v>827</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8033,7 +8129,7 @@
         <v>829</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8044,7 +8140,7 @@
         <v>831</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8052,32 +8148,32 @@
         <v>832</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>431</v>
+        <v>833</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>836</v>
+        <v>435</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8088,7 +8184,7 @@
         <v>838</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8099,7 +8195,7 @@
         <v>840</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8110,7 +8206,7 @@
         <v>842</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8121,7 +8217,7 @@
         <v>844</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8132,7 +8228,7 @@
         <v>846</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8143,7 +8239,7 @@
         <v>848</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8154,7 +8250,7 @@
         <v>850</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8165,7 +8261,7 @@
         <v>852</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8173,21 +8269,21 @@
         <v>853</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>819</v>
+        <v>854</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>856</v>
+        <v>823</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8195,21 +8291,21 @@
         <v>857</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>858</v>
+        <v>823</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>856</v>
+        <v>823</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B422" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="B422" s="1" t="s">
+      <c r="C422" s="1" t="s">
         <v>860</v>
-      </c>
-      <c r="C422" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8220,7 +8316,7 @@
         <v>862</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8231,7 +8327,7 @@
         <v>864</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8242,7 +8338,7 @@
         <v>866</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8253,7 +8349,7 @@
         <v>868</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8264,7 +8360,7 @@
         <v>870</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8275,7 +8371,7 @@
         <v>872</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8286,7 +8382,7 @@
         <v>874</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8297,7 +8393,7 @@
         <v>876</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8307,6 +8403,9 @@
       <c r="B431" s="1" t="s">
         <v>878</v>
       </c>
+      <c r="C431" s="1" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="s">
@@ -8315,6 +8414,9 @@
       <c r="B432" s="1" t="s">
         <v>880</v>
       </c>
+      <c r="C432" s="1" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
@@ -8633,17 +8735,14 @@
         <v>959</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>834</v>
+        <v>960</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>961</v>
-      </c>
-      <c r="C473" s="1" t="s">
         <v>962</v>
       </c>
     </row>
@@ -8652,14 +8751,17 @@
         <v>963</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>964</v>
+        <v>838</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="B475" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="B475" s="1" t="s">
+      <c r="C475" s="1" t="s">
         <v>966</v>
       </c>
     </row>
@@ -9140,79 +9242,79 @@
         <v>1085</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>958</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="1" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="1" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="1" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="1" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="1" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="1" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="1" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="1" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="1" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>1103</v>
+        <v>962</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9478,79 +9580,79 @@
       <c r="B577" s="1" t="s">
         <v>1169</v>
       </c>
-      <c r="C577" s="1" t="s">
-        <v>1170</v>
-      </c>
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B578" s="1" t="s">
         <v>1171</v>
-      </c>
-      <c r="B578" s="1" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B579" s="1" t="s">
         <v>1173</v>
-      </c>
-      <c r="B579" s="1" t="s">
-        <v>1174</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B580" s="1" t="s">
         <v>1175</v>
-      </c>
-      <c r="B580" s="1" t="s">
-        <v>1176</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B581" s="1" t="s">
         <v>1177</v>
-      </c>
-      <c r="B581" s="1" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B582" s="1" t="s">
         <v>1179</v>
-      </c>
-      <c r="B582" s="1" t="s">
-        <v>1180</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B583" s="1" t="s">
         <v>1181</v>
-      </c>
-      <c r="B583" s="1" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B584" s="1" t="s">
         <v>1183</v>
-      </c>
-      <c r="B584" s="1" t="s">
-        <v>1184</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B585" s="1" t="s">
         <v>1185</v>
-      </c>
-      <c r="B585" s="1" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B586" s="1" t="s">
         <v>1187</v>
       </c>
-      <c r="B586" s="1" t="s">
+      <c r="C586" s="1" t="s">
         <v>1188</v>
       </c>
     </row>
@@ -9655,143 +9757,143 @@
         <v>1213</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>43</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="1" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="1" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="1" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="1" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="1" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="1" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="1" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="1" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="1" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="1" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>1247</v>
+        <v>45</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9888,6 +9990,142 @@
       </c>
       <c r="B628" s="1" t="s">
         <v>1271</v>
+      </c>
+    </row>
+    <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A629" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A630" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A631" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B631" s="1" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A632" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A633" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A634" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B634" s="1" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A635" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A636" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A637" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B637" s="1" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A638" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B638" s="1" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A639" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B639" s="1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A640" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B640" s="1" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A641" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B641" s="1" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A642" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B642" s="1" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B643" s="1" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A644" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B644" s="1" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A645" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B645" s="1" t="s">
+        <v>1305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>